<commit_message>
Version 1.0 - works
</commit_message>
<xml_diff>
--- a/ExcelAnalyzer/Kontrol dokument.xlsx
+++ b/ExcelAnalyzer/Kontrol dokument.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laal_k\git\ExcelAnalyser\ExcelAnalyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lasse\git\ExcelAnalyser\ExcelAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3E1A31EA-4BE5-4C2B-B92B-EC235B96636B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC20408D-7024-46F0-9EED-430925079DD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1" xr2:uid="{530BD2B5-3412-4099-8AAB-C1E96B93769E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{530BD2B5-3412-4099-8AAB-C1E96B93769E}"/>
   </bookViews>
   <sheets>
     <sheet name="Indstillinger" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Gengående oplysninger - Android" sheetId="5" r:id="rId3"/>
     <sheet name="Data modifikation" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
   <si>
     <t>Måned</t>
   </si>
@@ -93,12 +93,6 @@
     <t>Kolonne 2</t>
   </si>
   <si>
-    <t>Bruger</t>
-  </si>
-  <si>
-    <t>Bruger - Total</t>
-  </si>
-  <si>
     <t>Total - brugere</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Sessioner</t>
   </si>
   <si>
-    <t>Sessioner - Total</t>
-  </si>
-  <si>
     <t>Sessioner / Sessioner - Total</t>
   </si>
   <si>
@@ -132,12 +123,6 @@
     <t>Erstatningsnavn</t>
   </si>
   <si>
-    <t>section_</t>
-  </si>
-  <si>
-    <t>section:</t>
-  </si>
-  <si>
     <t>Omdøb variabel</t>
   </si>
   <si>
@@ -156,9 +141,6 @@
     <t>IOS</t>
   </si>
   <si>
-    <t>Google Analytics</t>
-  </si>
-  <si>
     <t>Navn på output excel fil</t>
   </si>
   <si>
@@ -174,9 +156,6 @@
     <t>MAP:SELECT:Vejarbejde</t>
   </si>
   <si>
-    <t>MAP:SELECT:Vejarbejder</t>
-  </si>
-  <si>
     <t>Variabel 2 (Lægges til variabel 1 og frasorteres fra dataene)</t>
   </si>
   <si>
@@ -210,16 +189,22 @@
     <t>typeNameForSumOfVariables</t>
   </si>
   <si>
-    <t>IOS: Total - brugere</t>
-  </si>
-  <si>
-    <t>IOS: Antal sessioner</t>
-  </si>
-  <si>
-    <t>IOS: asdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">Antal sessioner </t>
+  </si>
+  <si>
+    <t>Antal sessioner</t>
+  </si>
+  <si>
+    <t>SCREEN:START:MainActivity</t>
+  </si>
+  <si>
+    <t>SCREEN:START:MainActivityasdf</t>
+  </si>
+  <si>
+    <t>WEBCAM;OPEN;(not set)</t>
+  </si>
+  <si>
+    <t>Brugere</t>
   </si>
 </sst>
 </file>
@@ -289,7 +274,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,7 +312,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -433,7 +418,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +571,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,76 +595,76 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B96F26-D742-4884-81ED-12C6D8394ABC}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,13 +701,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,10 +1332,14 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E37"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1360,13 +1349,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0F28D5-71A4-479A-B873-97608DCFFB51}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,7 +1990,7 @@
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="50.5703125" bestFit="1" customWidth="1"/>
@@ -2009,13 +1998,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2032,56 +2021,56 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Trafikkort - add on startet.
</commit_message>
<xml_diff>
--- a/ExcelAnalyzer/Kontrol dokument.xlsx
+++ b/ExcelAnalyzer/Kontrol dokument.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laal_k\git\ExcelAnalyser\ExcelAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D1F0FC1A-315D-47DE-96D3-2210E1A42BC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{205EA72B-F22B-43DB-9F14-B6693BCC95DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{530BD2B5-3412-4099-8AAB-C1E96B93769E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{530BD2B5-3412-4099-8AAB-C1E96B93769E}"/>
   </bookViews>
   <sheets>
     <sheet name="Indstillinger" sheetId="1" r:id="rId1"/>
     <sheet name="Gengående oplysninger" sheetId="5" r:id="rId2"/>
     <sheet name="Data modifikation" sheetId="3" r:id="rId3"/>
+    <sheet name="Data modifikation 2" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Indstillingsnavn</t>
   </si>
@@ -149,6 +150,9 @@
     <t>Brugere</t>
   </si>
   <si>
+    <t>Google Analytics - Trafikinfo</t>
+  </si>
+  <si>
     <t>Fil</t>
   </si>
   <si>
@@ -179,7 +183,22 @@
     <t>2018_09 Sep</t>
   </si>
   <si>
-    <t>Google Analytics - Trafikkort</t>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Opret separat ark for værdier over</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?utm_source=danwest.de&amp;utm_campaign=3ec1f9fb03-EMAIL_CAMPAIGN_2018_06_11_08</t>
+  </si>
+  <si>
+    <t>Summér og slet (hændelseskategori)</t>
+  </si>
+  <si>
+    <t>Variabel slut navn (bibeholdes)</t>
+  </si>
+  <si>
+    <t>Variabel der starter med:</t>
   </si>
 </sst>
 </file>
@@ -568,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9053337-8509-4929-97A0-4E6C284783EF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +667,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -688,7 +707,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -699,7 +718,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -710,7 +729,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -721,7 +740,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -732,7 +751,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -743,7 +762,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -754,7 +773,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -765,7 +784,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -776,7 +795,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -787,7 +806,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -914,7 +933,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,4 +1048,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D866B0EF-5A57-4881-BDF4-4352ECFC5504}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="116.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sum category function added
</commit_message>
<xml_diff>
--- a/ExcelAnalyzer/Kontrol dokument.xlsx
+++ b/ExcelAnalyzer/Kontrol dokument.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laal_k\git\ExcelAnalyser\ExcelAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{205EA72B-F22B-43DB-9F14-B6693BCC95DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7EB2D19B-C58D-4460-A93C-402D7E3C2202}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{530BD2B5-3412-4099-8AAB-C1E96B93769E}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Indstillingsnavn</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>Variabel der starter med:</t>
+  </si>
+  <si>
+    <t>Ekskluder værdier der slutter med: (Separer med ;)</t>
+  </si>
+  <si>
+    <t>GroupA,GroupG;GroupA1</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/index.html?visiblegroups</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/index.html?usertype=2</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/index.html?usertype=3</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/index.html?visibleGroups=GroupA1</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/index.html?lat</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?gclid</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?utm_medium=newsletter_ubivox&amp;utm_source=20180308_Sibirisk%20vinter%20skabte%20travlhed%20for%20sneryddere%20og%20saltspredere&amp;utm_campaign=Sibirisk%20vinter%20skabte%20travlhed%20for%20sneryddere%20og%20saltspredere</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?utm_medium=newsletter_ubivox&amp;utm_source=20180308_Sibirisk%20vinter</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/index.html?show</t>
   </si>
 </sst>
 </file>
@@ -209,7 +242,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _k_r_._-;\-* #,##0\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +271,14 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -256,12 +297,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,9 +311,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Link" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
@@ -933,7 +977,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +1043,12 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1045,23 +1095,26 @@
       <c r="D14" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{6D1977C5-CCE3-45C0-BACF-B280662CE129}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D866B0EF-5A57-4881-BDF4-4352ECFC5504}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="116.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="116.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1080,20 +1133,98 @@
       <c r="B2" t="s">
         <v>56</v>
       </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
       <c r="E2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>53</v>
       </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{BF640B75-C171-441D-8106-C748E5CFFA95}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{897AEA01-A44B-4D4F-BB8E-70019B8E0FEE}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{D7553258-B824-4245-9010-CB8EB319E6CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CSVReader is now closed after use.
</commit_message>
<xml_diff>
--- a/ExcelAnalyzer/Kontrol dokument.xlsx
+++ b/ExcelAnalyzer/Kontrol dokument.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laal_k\git\ExcelAnalyser\ExcelAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5CFE1295-31B0-46BF-9B87-A5DE0FF87DE1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EAFE06-B9B2-40BE-A90E-13EFCDBF6C4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{530BD2B5-3412-4099-8AAB-C1E96B93769E}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="135">
   <si>
     <t>Indstillingsnavn</t>
   </si>
@@ -267,12 +267,6 @@
     <t>Google Analytics - Trafikkort</t>
   </si>
   <si>
-    <t>layer_id_19</t>
-  </si>
-  <si>
-    <t>19_Vejr</t>
-  </si>
-  <si>
     <t>11_Live Trafik</t>
   </si>
   <si>
@@ -337,6 +331,108 @@
   </si>
   <si>
     <t>8_Samkørselspladser</t>
+  </si>
+  <si>
+    <t>layer_id_19L</t>
+  </si>
+  <si>
+    <t>19_Vejarbejde Fremtid</t>
+  </si>
+  <si>
+    <t>layer_id_19K</t>
+  </si>
+  <si>
+    <t>19_Vejarbejde Fremtid spærret vej</t>
+  </si>
+  <si>
+    <t>layer_id_19B</t>
+  </si>
+  <si>
+    <t>layer_id_19C</t>
+  </si>
+  <si>
+    <t>19_Nuværende vejarbejde</t>
+  </si>
+  <si>
+    <t>layer_id_19O</t>
+  </si>
+  <si>
+    <t>19_Fremtidig trafikmelding</t>
+  </si>
+  <si>
+    <t>19_Vejarbejde spærring vej</t>
+  </si>
+  <si>
+    <t>layer_id_19A</t>
+  </si>
+  <si>
+    <t>19_Spærret vej</t>
+  </si>
+  <si>
+    <t>layer_id_19Q</t>
+  </si>
+  <si>
+    <t>19_Andre fremtidig traffikmelding</t>
+  </si>
+  <si>
+    <t>layer_id_19J</t>
+  </si>
+  <si>
+    <t>19_Fremtidig spærret vej</t>
+  </si>
+  <si>
+    <t>layer_id_19F</t>
+  </si>
+  <si>
+    <t>19_Nuværende traffik melding</t>
+  </si>
+  <si>
+    <t>layer_id_19I</t>
+  </si>
+  <si>
+    <t>19_Nuværende kø melding</t>
+  </si>
+  <si>
+    <t>layer_id_19D</t>
+  </si>
+  <si>
+    <t>19_Glatføre melding</t>
+  </si>
+  <si>
+    <t>layer_id_19E</t>
+  </si>
+  <si>
+    <t>19_Sne melding</t>
+  </si>
+  <si>
+    <t>19_Kraftig vind</t>
+  </si>
+  <si>
+    <t>layer_id_19G</t>
+  </si>
+  <si>
+    <t>19_Andre trafik melding</t>
+  </si>
+  <si>
+    <t>layer_id_19H</t>
+  </si>
+  <si>
+    <t>2018_10 Okt</t>
+  </si>
+  <si>
+    <t>2018_12 Dec</t>
+  </si>
+  <si>
+    <t>2018_11 Nov</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?fbclid</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?type=html&amp;tags=%5bl_sID_Afd%20073060%5d%5bpp_playlist%5d&amp;p_playlist&amp;SOC=1&amp;BC=%2523FFF&amp;dur=360000&amp;cnl=1&amp;indexI=1295657&amp;fps=0&amp;res=0x0&amp;path=PostNord%20Danmark%20Logistic%20ZMP%5c%5bpp%5d%5c%5bpp_campaigns%5d%5cPostNord%20DK%20-%20Logistic%20-%20Trafikkort%20Vejdirektoratet%5cPostNord%20DK%20-%20Logistic%20-%20Trafikkort%20Vejdirektoratet%20files%5cVejdirektoratet.url</t>
+  </si>
+  <si>
+    <t>https://trafikkort.vejdirektoratet.dk/?type=PostnordRedirect</t>
   </si>
 </sst>
 </file>
@@ -347,7 +443,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _k_r_._-;\-* #,##0\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +480,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -408,7 +510,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,6 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -446,7 +549,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -484,7 +587,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -590,7 +693,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -850,7 +953,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,10 +979,10 @@
         <v>41</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>121468</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>332526</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -887,10 +990,10 @@
         <v>42</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>248064</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>584960</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,10 +1001,10 @@
         <v>43</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>319542</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>779025</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -909,10 +1012,10 @@
         <v>44</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>122484</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>271609</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,10 +1023,10 @@
         <v>45</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>131571</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>295485</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,10 +1034,10 @@
         <v>46</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>144255</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>316910</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -942,10 +1045,10 @@
         <v>47</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>154064</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>321222</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -953,10 +1056,10 @@
         <v>48</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>144318</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>305147</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,23 +1067,44 @@
         <v>49</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>143968</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>311316</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11">
+        <v>159614</v>
+      </c>
+      <c r="C11">
+        <v>358498</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <v>130709</v>
+      </c>
+      <c r="C12">
+        <v>320150</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>156497</v>
+      </c>
+      <c r="C13">
+        <v>374335</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
@@ -1080,6 +1204,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1216,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D866B0EF-5A57-4881-BDF4-4352ECFC5504}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,10 +1403,10 @@
         <v>69</v>
       </c>
       <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
         <v>79</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1295,10 +1420,10 @@
         <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1315,10 +1440,10 @@
         <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1332,7 +1457,7 @@
         <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G6" t="s">
         <v>83</v>
@@ -1349,10 +1474,10 @@
         <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1366,7 +1491,7 @@
         <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
         <v>84</v>
@@ -1383,10 +1508,10 @@
         <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1400,14 +1525,14 @@
         <v>69</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1417,13 +1542,19 @@
         <v>69</v>
       </c>
       <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
       <c r="E12" t="s">
         <v>69</v>
       </c>
@@ -1434,15 +1565,21 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="E13" t="s">
         <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1453,7 +1590,7 @@
         <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,10 +1598,10 @@
         <v>69</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1472,10 +1609,10 @@
         <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
@@ -1483,18 +1620,164 @@
         <v>69</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" t="s">
-        <v>99</v>
+      <c r="G21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1502,8 +1785,11 @@
     <hyperlink ref="A3" r:id="rId1" xr:uid="{BF640B75-C171-441D-8106-C748E5CFFA95}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{897AEA01-A44B-4D4F-BB8E-70019B8E0FEE}"/>
     <hyperlink ref="B11" r:id="rId3" xr:uid="{D7553258-B824-4245-9010-CB8EB319E6CB}"/>
+    <hyperlink ref="B13" r:id="rId4" display="https://trafikkort.vejdirektoratet.dk/?type=html&amp;tags=%5bl_sID_Afd%20073060%5d%5bpp_playlist%5d&amp;p_playlist&amp;SOC=1&amp;BC=%2523FFF&amp;dur=360000&amp;cnl=1&amp;indexI=1295657&amp;fps=0&amp;res=0x0&amp;path=PostNord%20Danmark%20Logistic%20ZMP%5c%5bpp%5d%5c%5bpp_campaigns%5d%5cPostNord%20DK%20-%20Logistic%20-%20Trafikkort%20Vejdirektoratet%5cPostNord%20DK%20-%20Logistic%20-%20Trafikkort%20Vejdirektoratet%20files%5cVejdirektoratet.url" xr:uid="{1484C866-4BD0-4B87-9084-AD657E5B01F3}"/>
+    <hyperlink ref="A11" r:id="rId5" xr:uid="{B2D7163B-6C97-4732-AEA5-E6D7F1538C7E}"/>
+    <hyperlink ref="A13" r:id="rId6" xr:uid="{345F2A2C-2664-4C4E-8EB1-BCBC0C358C67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>